<commit_message>
tasks hid in excel
</commit_message>
<xml_diff>
--- a/content/Excel_data.xlsx
+++ b/content/Excel_data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria/Desktop/UBC/ResearchCommons/Excel workshops/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria/Documents/GitHub/excel1/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD0EB7D-7D65-1B44-B9A9-5A07088426A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB59FE44-8FEF-C74E-B712-FC5FF280E41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
-    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Summary" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -823,82 +823,82 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1455,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -1484,15 +1484,15 @@
       <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
@@ -1513,7 +1513,7 @@
       <c r="C4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="55" t="s">
         <v>70</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -1540,7 +1540,7 @@
       <c r="E5" s="3">
         <v>28</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="53" t="s">
         <v>157</v>
       </c>
       <c r="G5" s="3">
@@ -1774,7 +1774,7 @@
       <c r="E15" s="3">
         <v>128</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="53" t="s">
         <v>157</v>
       </c>
       <c r="G15" s="3">
@@ -2128,7 +2128,7 @@
       <c r="F30" s="3">
         <v>2</v>
       </c>
-      <c r="G30" s="77" t="s">
+      <c r="G30" s="53" t="s">
         <v>157</v>
       </c>
       <c r="H30" s="8" t="str">
@@ -2200,7 +2200,7 @@
       <c r="F33" s="3">
         <v>611</v>
       </c>
-      <c r="G33" s="77" t="s">
+      <c r="G33" s="53" t="s">
         <v>157</v>
       </c>
       <c r="H33" s="8" t="str">
@@ -2242,7 +2242,7 @@
       <c r="E35" s="3">
         <v>54</v>
       </c>
-      <c r="F35" s="77" t="s">
+      <c r="F35" s="53" t="s">
         <v>157</v>
       </c>
       <c r="G35" s="3">
@@ -2640,13 +2640,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
@@ -2666,102 +2666,102 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
     </row>
     <row r="5" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="58" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="61">
         <v>2</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
     </row>
     <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
     </row>
     <row r="8" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="60">
         <v>3</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
     </row>
     <row r="10" spans="1:6" s="24" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="74" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="75">
         <v>5</v>
       </c>
-      <c r="E10" s="68"/>
+      <c r="E10" s="78"/>
     </row>
     <row r="11" spans="1:6" s="24" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="69"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="79"/>
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="32" t="s">
         <v>17</v>
       </c>
@@ -2785,10 +2785,10 @@
       <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="57" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2799,8 +2799,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="26" t="s">
         <v>86</v>
       </c>
@@ -2812,16 +2812,16 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="57" t="s">
         <v>88</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="60">
         <v>3</v>
       </c>
       <c r="E16" s="43" t="s">
@@ -2829,45 +2829,45 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="70" t="s">
+      <c r="D17" s="61"/>
+      <c r="E17" s="63" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="70"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="63"/>
     </row>
     <row r="19" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="57" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="60">
         <v>5</v>
       </c>
       <c r="E20" s="45" t="s">
@@ -2875,45 +2875,45 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="66"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="70" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="63" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="55"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="71"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="67"/>
     </row>
     <row r="23" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
     </row>
     <row r="24" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="71" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="59">
+      <c r="D24" s="71">
         <v>5</v>
       </c>
       <c r="E24" s="46" t="s">
@@ -2921,76 +2921,76 @@
       </c>
     </row>
     <row r="25" spans="1:6" s="24" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="28" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="24" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="72" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="47" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="24" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="60"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="32" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="57" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="60">
         <v>3</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="57" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="89" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="78" t="s">
+      <c r="D29" s="62"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="54" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="57" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="60">
         <v>10</v>
       </c>
       <c r="E30" s="42" t="s">
@@ -2998,44 +2998,44 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
-      <c r="B31" s="66"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="67"/>
+      <c r="D31" s="61"/>
       <c r="E31" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="F31" s="78" t="s">
+      <c r="F31" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="57"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="F32" s="78" t="s">
+      <c r="F32" s="54" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="60">
         <v>10</v>
       </c>
       <c r="E33" s="42" t="s">
@@ -3043,16 +3043,16 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="57"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="78" t="s">
+      <c r="F34" s="54" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3072,24 +3072,24 @@
       <c r="E35" s="48"/>
     </row>
     <row r="36" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
     </row>
     <row r="37" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="58" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="67">
+      <c r="D37" s="61">
         <v>2</v>
       </c>
       <c r="E37" s="44" t="s">
@@ -3097,36 +3097,36 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="66"/>
-      <c r="B38" s="66"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="70" t="s">
+      <c r="D38" s="61"/>
+      <c r="E38" s="63" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="59"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="57"/>
-      <c r="E39" s="71"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="67"/>
     </row>
     <row r="40" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="57" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="56">
+      <c r="D40" s="60">
         <v>10</v>
       </c>
       <c r="E40" s="42" t="s">
@@ -3134,58 +3134,58 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="66"/>
-      <c r="B41" s="66"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="67"/>
+      <c r="D41" s="61"/>
       <c r="E41" s="49" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="66"/>
-      <c r="B42" s="66"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="67"/>
-      <c r="E42" s="75" t="s">
+      <c r="D42" s="61"/>
+      <c r="E42" s="68" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
-      <c r="B43" s="66"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="75"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="68"/>
     </row>
     <row r="44" spans="1:6" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="59"/>
       <c r="C44" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="57"/>
+      <c r="D44" s="62"/>
       <c r="E44" s="26" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54" t="s">
+      <c r="A45" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="57" t="s">
         <v>63</v>
       </c>
       <c r="C45" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="56">
+      <c r="D45" s="60">
         <v>5</v>
       </c>
       <c r="E45" s="42" t="s">
@@ -3193,93 +3193,93 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="66"/>
-      <c r="B46" s="66"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="67"/>
-      <c r="E46" s="70" t="s">
+      <c r="D46" s="61"/>
+      <c r="E46" s="63" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="66"/>
-      <c r="B47" s="66"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="58"/>
       <c r="C47" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="67"/>
-      <c r="E47" s="70"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="63"/>
     </row>
     <row r="48" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="66"/>
-      <c r="B48" s="66"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="58"/>
       <c r="C48" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="67"/>
+      <c r="D48" s="61"/>
       <c r="E48" s="51" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
-      <c r="B49" s="55"/>
+      <c r="A49" s="59"/>
+      <c r="B49" s="59"/>
       <c r="C49" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="57"/>
+      <c r="D49" s="62"/>
       <c r="E49" s="21" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="57" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D50" s="56">
+      <c r="D50" s="60">
         <v>10</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F50" s="78" t="s">
+      <c r="F50" s="54" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="74"/>
-      <c r="B51" s="74"/>
+      <c r="A51" s="65"/>
+      <c r="B51" s="65"/>
       <c r="C51" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="65"/>
-      <c r="E51" s="76"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="66"/>
     </row>
     <row r="52" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="65"/>
       <c r="C52" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="76"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="66"/>
     </row>
     <row r="53" spans="1:6" ht="398" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
-      <c r="B53" s="74"/>
+      <c r="A53" s="65"/>
+      <c r="B53" s="65"/>
       <c r="C53" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="65"/>
-      <c r="E53" s="76"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="66"/>
     </row>
     <row r="54" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -3309,6 +3309,54 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="B45:B49"/>
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="D45:D49"/>
@@ -3317,54 +3365,6 @@
     <mergeCell ref="B50:B53"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="D40:D44"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -3386,7 +3386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>